<commit_message>
EPBDS-7344 Issue with field parsing in Data/Test tables
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CollectionsInDataTablesAndTestTables.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CollectionsInDataTablesAndTestTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605"/>
   </bookViews>
   <sheets>
     <sheet name="MultiRow" sheetId="1" r:id="rId1"/>
@@ -221,15 +221,6 @@
     <t>Data List listData</t>
   </si>
   <si>
-    <t>[0]:String</t>
-  </si>
-  <si>
-    <t>[3]:Integer</t>
-  </si>
-  <si>
-    <t>["key1"]:String</t>
-  </si>
-  <si>
     <t>["key2"]:Integer</t>
   </si>
   <si>
@@ -294,6 +285,15 @@
   </si>
   <si>
     <t>&gt; mapData</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 3 ] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 0 ] : String </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ "key1" ] : String </t>
   </si>
 </sst>
 </file>
@@ -666,74 +666,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1095,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:M156"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
       <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
@@ -1131,13 +1131,13 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1189,7 +1189,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
@@ -1210,7 +1210,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="30" t="s">
         <v>1</v>
       </c>
@@ -1229,11 +1229,11 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="30" t="s">
@@ -1248,11 +1248,11 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="30" t="s">
         <v>1</v>
       </c>
@@ -1265,10 +1265,10 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="43">
-        <v>2</v>
-      </c>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="41">
+        <v>2</v>
+      </c>
+      <c r="C14" s="40" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="30" t="s">
@@ -1286,8 +1286,8 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="43"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="30" t="s">
         <v>9</v>
       </c>
@@ -1330,13 +1330,13 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="48"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1388,7 +1388,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="30" t="s">
@@ -1409,7 +1409,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="43"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="30" t="s">
         <v>1</v>
       </c>
@@ -1428,11 +1428,11 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="43"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="30" t="s">
@@ -1447,11 +1447,11 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="43"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="39"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="30" t="s">
         <v>1</v>
       </c>
@@ -1464,10 +1464,10 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="43">
-        <v>2</v>
-      </c>
-      <c r="C25" s="39" t="s">
+      <c r="B25" s="41">
+        <v>2</v>
+      </c>
+      <c r="C25" s="40" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="30" t="s">
@@ -1485,8 +1485,8 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="43"/>
-      <c r="C26" s="39"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="30" t="s">
         <v>9</v>
       </c>
@@ -1582,10 +1582,10 @@
       <c r="J35" s="1"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="48"/>
+      <c r="C38" s="46"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
@@ -1634,10 +1634,10 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="46" t="s">
+      <c r="B47" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="49"/>
+      <c r="C47" s="45"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
@@ -1686,10 +1686,10 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C55" s="49"/>
+      <c r="C55" s="45"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -1730,11 +1730,11 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="46" t="s">
+      <c r="B62" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C62" s="46"/>
-      <c r="D62" s="50"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="47"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1809,11 +1809,11 @@
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="46" t="s">
+      <c r="B73" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C73" s="46"/>
-      <c r="D73" s="46"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
@@ -1872,10 +1872,10 @@
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="46" t="s">
+      <c r="B81" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C81" s="46"/>
+      <c r="C81" s="44"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
@@ -1924,10 +1924,10 @@
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="46" t="s">
+      <c r="B89" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C89" s="46"/>
+      <c r="C89" s="44"/>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -1976,10 +1976,10 @@
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="46" t="s">
+      <c r="B97" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C97" s="46"/>
+      <c r="C97" s="44"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
@@ -2020,13 +2020,13 @@
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="41" t="s">
+      <c r="B105" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C105" s="41"/>
-      <c r="D105" s="41"/>
-      <c r="E105" s="42"/>
-      <c r="F105" s="42"/>
+      <c r="C105" s="42"/>
+      <c r="D105" s="42"/>
+      <c r="E105" s="43"/>
+      <c r="F105" s="43"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
@@ -2061,7 +2061,7 @@
       <c r="F107" s="4"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B108" s="39" t="s">
+      <c r="B108" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C108" s="28" t="s">
@@ -2073,12 +2073,12 @@
       <c r="E108" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F108" s="39">
+      <c r="F108" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" s="39"/>
+      <c r="B109" s="40"/>
       <c r="C109" s="28" t="s">
         <v>9</v>
       </c>
@@ -2088,11 +2088,11 @@
       <c r="E109" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F109" s="39"/>
+      <c r="F109" s="40"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B110" s="39"/>
-      <c r="C110" s="39" t="s">
+      <c r="B110" s="40"/>
+      <c r="C110" s="40" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="28" t="s">
@@ -2101,21 +2101,21 @@
       <c r="E110" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F110" s="39"/>
+      <c r="F110" s="40"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B111" s="39"/>
-      <c r="C111" s="39"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="40"/>
       <c r="D111" s="28" t="s">
         <v>1</v>
       </c>
       <c r="E111" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F111" s="39"/>
+      <c r="F111" s="40"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="39" t="s">
+      <c r="B112" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C112" s="28" t="s">
@@ -2127,12 +2127,12 @@
       <c r="E112" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F112" s="39">
+      <c r="F112" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="43"/>
+      <c r="B113" s="41"/>
       <c r="C113" s="28" t="s">
         <v>9</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="E113" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F113" s="39"/>
+      <c r="F113" s="40"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="28" t="s">
@@ -2162,13 +2162,13 @@
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B118" s="41" t="s">
+      <c r="B118" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C118" s="41"/>
-      <c r="D118" s="41"/>
-      <c r="E118" s="42"/>
-      <c r="F118" s="42"/>
+      <c r="C118" s="42"/>
+      <c r="D118" s="42"/>
+      <c r="E118" s="43"/>
+      <c r="F118" s="43"/>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
@@ -2203,7 +2203,7 @@
       <c r="F120" s="4"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="39" t="s">
+      <c r="B121" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C121" s="28" t="s">
@@ -2215,12 +2215,12 @@
       <c r="E121" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F121" s="39">
+      <c r="F121" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="39"/>
+      <c r="B122" s="40"/>
       <c r="C122" s="28" t="s">
         <v>9</v>
       </c>
@@ -2230,11 +2230,11 @@
       <c r="E122" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F122" s="39"/>
+      <c r="F122" s="40"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="39"/>
-      <c r="C123" s="39" t="s">
+      <c r="B123" s="40"/>
+      <c r="C123" s="40" t="s">
         <v>8</v>
       </c>
       <c r="D123" s="29" t="s">
@@ -2243,21 +2243,21 @@
       <c r="E123" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F123" s="39"/>
+      <c r="F123" s="40"/>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="39"/>
-      <c r="C124" s="39"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
       <c r="D124" s="29" t="s">
         <v>1</v>
       </c>
       <c r="E124" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F124" s="39"/>
+      <c r="F124" s="40"/>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B125" s="39" t="s">
+      <c r="B125" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C125" s="28" t="s">
@@ -2269,12 +2269,12 @@
       <c r="E125" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F125" s="39">
+      <c r="F125" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="39"/>
+      <c r="B126" s="40"/>
       <c r="C126" s="28" t="s">
         <v>9</v>
       </c>
@@ -2284,7 +2284,7 @@
       <c r="E126" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F126" s="39"/>
+      <c r="F126" s="40"/>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="27" t="s">
@@ -2324,16 +2324,16 @@
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B139" s="40" t="s">
+      <c r="B139" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C139" s="41"/>
-      <c r="D139" s="41"/>
-      <c r="E139" s="41"/>
-      <c r="F139" s="41"/>
-      <c r="G139" s="41"/>
-      <c r="H139" s="41"/>
-      <c r="I139" s="42"/>
+      <c r="C139" s="42"/>
+      <c r="D139" s="42"/>
+      <c r="E139" s="42"/>
+      <c r="F139" s="42"/>
+      <c r="G139" s="42"/>
+      <c r="H139" s="42"/>
+      <c r="I139" s="43"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" s="2" t="s">
@@ -2386,7 +2386,7 @@
       <c r="I141" s="4"/>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B142" s="39" t="s">
+      <c r="B142" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C142" s="28" t="s">
@@ -2401,12 +2401,12 @@
       <c r="F142" s="28"/>
       <c r="G142" s="28"/>
       <c r="H142" s="28"/>
-      <c r="I142" s="39">
+      <c r="I142" s="40">
         <v>4</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B143" s="39"/>
+      <c r="B143" s="40"/>
       <c r="C143" s="28" t="s">
         <v>9</v>
       </c>
@@ -2419,11 +2419,11 @@
       <c r="F143" s="28"/>
       <c r="G143" s="28"/>
       <c r="H143" s="28"/>
-      <c r="I143" s="39"/>
+      <c r="I143" s="40"/>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B144" s="39"/>
-      <c r="C144" s="39" t="s">
+      <c r="B144" s="40"/>
+      <c r="C144" s="40" t="s">
         <v>8</v>
       </c>
       <c r="D144" s="28" t="s">
@@ -2441,11 +2441,11 @@
       <c r="H144" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I144" s="39"/>
+      <c r="I144" s="40"/>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B145" s="39"/>
-      <c r="C145" s="39"/>
+      <c r="B145" s="40"/>
+      <c r="C145" s="40"/>
       <c r="D145" s="28" t="s">
         <v>1</v>
       </c>
@@ -2461,10 +2461,10 @@
       <c r="H145" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I145" s="39"/>
+      <c r="I145" s="40"/>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B146" s="39" t="s">
+      <c r="B146" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C146" s="28" t="s">
@@ -2485,12 +2485,12 @@
       <c r="H146" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I146" s="39">
+      <c r="I146" s="40">
         <v>3</v>
       </c>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B147" s="43"/>
+      <c r="B147" s="41"/>
       <c r="C147" s="28" t="s">
         <v>9</v>
       </c>
@@ -2503,7 +2503,7 @@
       <c r="F147" s="28"/>
       <c r="G147" s="28"/>
       <c r="H147" s="28"/>
-      <c r="I147" s="39"/>
+      <c r="I147" s="40"/>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B148" s="28" t="s">
@@ -2524,18 +2524,18 @@
       </c>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B150" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C150" s="51"/>
-      <c r="D150" s="51"/>
+      <c r="B150" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C150" s="39"/>
+      <c r="D150" s="39"/>
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B151" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C151" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D151" s="36" t="s">
         <v>2</v>
@@ -2543,20 +2543,20 @@
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B152" s="36" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C152" s="36"/>
       <c r="D152" s="36"/>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B153" s="36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C153" s="36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D153" s="36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>7</v>
       </c>
       <c r="C154" s="38" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D154" s="36" t="s">
         <v>7</v>
@@ -2575,7 +2575,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D155" s="36" t="s">
         <v>7</v>
@@ -2586,19 +2586,26 @@
         <v>7</v>
       </c>
       <c r="C156" s="38" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D156" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B150:D150"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="F112:F113"/>
-    <mergeCell ref="F121:F124"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="I142:I145"/>
+    <mergeCell ref="I146:I147"/>
+    <mergeCell ref="B139:I139"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="B118:F118"/>
@@ -2615,20 +2622,13 @@
     <mergeCell ref="B108:B111"/>
     <mergeCell ref="F108:F111"/>
     <mergeCell ref="C110:C111"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="I142:I145"/>
-    <mergeCell ref="I146:I147"/>
-    <mergeCell ref="B139:I139"/>
-    <mergeCell ref="B142:B145"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="B150:D150"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="F112:F113"/>
+    <mergeCell ref="F121:F124"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="C123:C124"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2638,8 +2638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,196 +2648,196 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="54"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
+      <c r="D5" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
+      <c r="D6" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="55"/>
+      <c r="I6" s="56"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="34">
         <v>1</v>
       </c>
-      <c r="D7" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="59"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="54"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="53" t="s">
+      <c r="D8" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="54"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="55" t="s">
+      <c r="D9" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="60"/>
+      <c r="C15" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="61"/>
-      <c r="I16" s="62"/>
+      <c r="D16" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="55"/>
+      <c r="I16" s="56"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
+      <c r="D17" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="55"/>
+      <c r="I17" s="56"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="34">
         <v>1</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53" t="s">
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="53"/>
-      <c r="I18" s="54"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="60"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53" t="s">
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="53"/>
-      <c r="I19" s="54"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="60"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56" t="s">
+      <c r="E20" s="57"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="56"/>
-      <c r="I20" s="57"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="58"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="52" t="s">
-        <v>73</v>
+      <c r="B34" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="61" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D35" s="36" t="s">
         <v>2</v>
@@ -2853,20 +2853,20 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C36" s="36"/>
       <c r="D36" s="36"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -2886,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -2902,16 +2902,23 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C44" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C45" s="37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="D16:F16"/>
@@ -2928,13 +2935,6 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>